<commit_message>
Update README.md to include HDF5 file handling and utility script for managing flux map data
</commit_message>
<xml_diff>
--- a/Real_Numbers.xlsx
+++ b/Real_Numbers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a4f1e474212067a/Pygrams/TFG_Script/DiffusionWithConsumption/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a4f1e474212067a/Pygrams/TFG_program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{DC6F77A5-F379-45E0-96D7-6D7EEF9E61B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B01533EC-3480-4AE1-AF41-169877C3A9E1}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{DC6F77A5-F379-45E0-96D7-6D7EEF9E61B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27CFC810-FC05-4437-AAE6-A2084603F72E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1C7316B5-0443-4532-9286-116E151C3214}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>1.7-2.4 µm in length</t>
   </si>
   <si>
-    <t>1–2 µm long</t>
-  </si>
-  <si>
     <t>Interaction Source</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>Marinobacter adhaerens</t>
+  </si>
+  <si>
+    <t>1.4–2 µm long</t>
   </si>
 </sst>
 </file>
@@ -222,10 +222,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -548,7 +544,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,34 +568,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
@@ -621,13 +617,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="H2" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>6</v>
@@ -654,7 +650,7 @@
         <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>12</v>
@@ -673,7 +669,7 @@
         <v>9</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -716,7 +712,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -732,13 +728,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -766,7 +762,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>